<commit_message>
Regenerate demo files using new option "connectPoints" for chocolate
</commit_message>
<xml_diff>
--- a/demo/Results_chocolate/Distance/Anova.xlsx
+++ b/demo/Results_chocolate/Distance/Anova.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="21" uniqueCount="18">
   <si>
     <t>Term</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>etaSqp</t>
+  </si>
+  <si>
+    <t>SMD</t>
   </si>
   <si>
     <t>effectSize</t>
@@ -109,7 +112,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -121,8 +124,9 @@
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
     <col min="5" max="5" width="13.7109375" customWidth="true"/>
     <col min="6" max="6" width="14.7109375" customWidth="true"/>
-    <col min="7" max="7" width="10" customWidth="true"/>
-    <col min="8" max="8" width="11.5703125" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="10" customWidth="true"/>
+    <col min="9" max="9" width="11.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -148,7 +152,10 @@
         <v>10</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -162,19 +169,22 @@
         <v>490</v>
       </c>
       <c r="D2" s="0">
-        <v>375858.88620146411</v>
+        <v>375858.88592197088</v>
       </c>
       <c r="E2" s="0">
         <v>0</v>
       </c>
       <c r="F2" s="0">
-        <v>0.99869801660649082</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
+        <v>0.99869801660552382</v>
+      </c>
+      <c r="G2" s="0">
+        <v>55.39165824783241</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -188,19 +198,22 @@
         <v>490</v>
       </c>
       <c r="D3" s="0">
-        <v>4.0090864672660222</v>
+        <v>4.0090864702492341</v>
       </c>
       <c r="E3" s="0">
-        <v>0.04580625202817179</v>
+        <v>0.045806251947808296</v>
       </c>
       <c r="F3" s="0">
-        <v>0.0081154103782495341</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>0.0081154103842393053</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0.18090670659715877</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -214,19 +227,22 @@
         <v>490</v>
       </c>
       <c r="D4" s="0">
-        <v>945.88974751950343</v>
+        <v>945.88974683159074</v>
       </c>
       <c r="E4" s="0">
         <v>0</v>
       </c>
       <c r="F4" s="0">
-        <v>0.65874817279914832</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>11</v>
+        <v>0.65874817263565988</v>
+      </c>
+      <c r="G4" s="0">
+        <v>2.7787675242321499</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -240,19 +256,22 @@
         <v>490</v>
       </c>
       <c r="D5" s="0">
-        <v>138.89344584665582</v>
+        <v>138.89344594999253</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
       </c>
       <c r="F5" s="0">
-        <v>0.22085370226695358</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>13</v>
+        <v>0.22085370239497912</v>
+      </c>
+      <c r="G5" s="0">
+        <v>1.0648117432538804</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>